<commit_message>
grotere resultaten voor jl
</commit_message>
<xml_diff>
--- a/meting WV jl.xlsx
+++ b/meting WV jl.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -448,976 +448,1318 @@
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
           <t>OM</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="0" t="inlineStr">
         <is>
           <t>EU</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="0" t="inlineStr">
         <is>
           <t>AX</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="0" t="inlineStr">
         <is>
           <t>HO</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="0" t="inlineStr">
         <is>
           <t>RO</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="0" t="inlineStr">
         <is>
           <t>n</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="0" t="inlineStr">
         <is>
           <t>NOT all times are in ms</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="0" t="inlineStr">
         <is>
           <t>eenheid om</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="0" t="inlineStr">
         <is>
           <t>eenheid eu</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="0" t="inlineStr">
         <is>
           <t>eenheid ax</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="0" t="inlineStr">
         <is>
           <t>eenheid ho</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="0" t="inlineStr">
         <is>
           <t>eenheid ro</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="0" t="inlineStr">
         <is>
           <t>2.632</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>2.109</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>1.440</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>2.091</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="0" t="inlineStr">
         <is>
           <t>1.674</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="0" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
+      <c r="H2" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="J2" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="K2" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="L2" s="0" t="inlineStr">
         <is>
           <t>μs</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="0" t="inlineStr">
         <is>
           <t>4.718</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>3.754</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>2.410</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>3.728</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="0" t="inlineStr">
         <is>
           <t>2.904</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="0" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
+      <c r="H3" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="I3" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="J3" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="K3" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="L3" s="0" t="inlineStr">
         <is>
           <t>μs</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="0" t="inlineStr">
         <is>
           <t>8.933</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>7.049</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>4.462</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>7.008</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="0" t="inlineStr">
         <is>
           <t>5.324</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="0" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
+      <c r="H4" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="K4" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="L4" s="0" t="inlineStr">
         <is>
           <t>μs</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="0" t="inlineStr">
         <is>
           <t>17.335</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>13.386</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>8.193</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>14.472</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="0" t="inlineStr">
         <is>
           <t>10.120</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="0" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
+      <c r="H5" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="I5" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="J5" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="K5" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="L5" s="0" t="inlineStr">
         <is>
           <t>μs</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="0" t="inlineStr">
         <is>
           <t>34.570</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>27.136</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>16.979</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="0" t="inlineStr">
         <is>
           <t>26.394</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="0" t="inlineStr">
         <is>
           <t>19.822</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="0" t="inlineStr">
         <is>
           <t>32</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
+      <c r="H6" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="I6" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="J6" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="K6" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="L6" s="0" t="inlineStr">
         <is>
           <t>μs</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="0" t="inlineStr">
         <is>
           <t>68.350</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
         <is>
           <t>53.644</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="0" t="inlineStr">
         <is>
           <t>31.073</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="0" t="inlineStr">
         <is>
           <t>51.825</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="0" t="inlineStr">
         <is>
           <t>39.040</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="0" t="inlineStr">
         <is>
           <t>64</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
+      <c r="H7" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="I7" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="J7" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="K7" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="L7" s="0" t="inlineStr">
         <is>
           <t>μs</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="0" t="inlineStr">
         <is>
           <t>136.266</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>106.863</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="0" t="inlineStr">
         <is>
           <t>61.319</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="0" t="inlineStr">
         <is>
           <t>103.643</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="0" t="inlineStr">
         <is>
           <t>83.527</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="0" t="inlineStr">
         <is>
           <t>128</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
+      <c r="H8" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="I8" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="J8" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="K8" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="L8" s="0" t="inlineStr">
         <is>
           <t>μs</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="0" t="inlineStr">
         <is>
           <t>272.036</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>214.717</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="0" t="inlineStr">
         <is>
           <t>122.588</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="0" t="inlineStr">
         <is>
           <t>207.386</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="0" t="inlineStr">
         <is>
           <t>154.394</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="0" t="inlineStr">
         <is>
           <t>256</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
+      <c r="H9" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="I9" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="J9" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="K9" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="L9" s="0" t="inlineStr">
         <is>
           <t>μs</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="0" t="inlineStr">
         <is>
           <t>543.605</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>429.076</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="0" t="inlineStr">
         <is>
           <t>242.779</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="0" t="inlineStr">
         <is>
           <t>413.202</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="0" t="inlineStr">
         <is>
           <t>308.273</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="0" t="inlineStr">
         <is>
           <t>512</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
+      <c r="H10" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="I10" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="J10" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="K10" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="L10" s="0" t="inlineStr">
         <is>
           <t>μs</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="0" t="inlineStr">
         <is>
           <t>1.089</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr">
         <is>
           <t>862.185</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="0" t="inlineStr">
         <is>
           <t>484.834</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>825.936</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="0" t="inlineStr">
         <is>
           <t>618.909</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="0" t="inlineStr">
         <is>
           <t>1024</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>μs</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
+      <c r="H11" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="I11" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="J11" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="K11" s="0" t="inlineStr">
+        <is>
+          <t>μs</t>
+        </is>
+      </c>
+      <c r="L11" s="0" t="inlineStr">
         <is>
           <t>μs</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="0" t="inlineStr">
         <is>
           <t>2.215</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>1.772</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="0" t="inlineStr">
         <is>
           <t>1.004</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="0" t="inlineStr">
         <is>
           <t>1.893</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" s="0" t="inlineStr">
         <is>
           <t>1.276</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="0" t="inlineStr">
         <is>
           <t>2048</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
+      <c r="H12" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="I12" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="J12" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="K12" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="L12" s="0" t="inlineStr">
         <is>
           <t>ms</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="0" t="inlineStr">
         <is>
           <t>4.690</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
         <is>
           <t>3.693</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>2.077</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="0" t="inlineStr">
         <is>
           <t>3.502</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" s="0" t="inlineStr">
         <is>
           <t>2.610</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" s="0" t="inlineStr">
         <is>
           <t>4096</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
+      <c r="H13" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="I13" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="J13" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="K13" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="L13" s="0" t="inlineStr">
         <is>
           <t>ms</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="0" t="inlineStr">
         <is>
           <t>9.516</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
         <is>
           <t>7.395</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>4.219</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="0" t="inlineStr">
         <is>
           <t>7.003</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" s="0" t="inlineStr">
         <is>
           <t>5.270</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" s="0" t="inlineStr">
         <is>
           <t>8192</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
+      <c r="H14" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="I14" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="J14" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="K14" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="L14" s="0" t="inlineStr">
         <is>
           <t>ms</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="0" t="inlineStr">
         <is>
           <t>19.809</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
         <is>
           <t>14.892</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>8.459</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="0" t="inlineStr">
         <is>
           <t>14.271</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" s="0" t="inlineStr">
         <is>
           <t>10.874</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" s="0" t="inlineStr">
         <is>
           <t>16384</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
+      <c r="H15" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="I15" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="J15" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="K15" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="L15" s="0" t="inlineStr">
         <is>
           <t>ms</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="0" t="inlineStr">
         <is>
           <t>42.698</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>30.705</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>17.447</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>34.049</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E16" s="0" t="inlineStr">
         <is>
           <t>23.989</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" s="0" t="inlineStr">
         <is>
           <t>32768</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
+      <c r="H16" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="I16" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="J16" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="K16" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="L16" s="0" t="inlineStr">
         <is>
           <t>ms</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="0" t="inlineStr">
         <is>
           <t>92.204</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>69.719</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>41.207</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D17" s="0" t="inlineStr">
         <is>
           <t>73.350</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E17" s="0" t="inlineStr">
         <is>
           <t>53.974</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" s="0" t="inlineStr">
         <is>
           <t>65536</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>ms</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>ms</t>
+      <c r="H17" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="I17" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="J17" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="K17" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="L17" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>209.412</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>122.214</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>74.623</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>137.305</t>
+        </is>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
+          <t>101.295</t>
+        </is>
+      </c>
+      <c r="F18" s="0" t="inlineStr">
+        <is>
+          <t>131072</t>
+        </is>
+      </c>
+      <c r="H18" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="I18" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="J18" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="K18" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="L18" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>391.310</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>253.089</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>169.385</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>305.994</t>
+        </is>
+      </c>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>228.302</t>
+        </is>
+      </c>
+      <c r="F19" s="0" t="inlineStr">
+        <is>
+          <t>262144</t>
+        </is>
+      </c>
+      <c r="H19" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="I19" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="J19" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="K19" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="L19" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>884.075</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>582.976</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>373.637</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>689.263</t>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t>541.185</t>
+        </is>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
+        <is>
+          <t>524288</t>
+        </is>
+      </c>
+      <c r="H20" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="I20" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="J20" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="K20" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="L20" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>1.999</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>1.285</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>877.359</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>1.507</t>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>1.189</t>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>1048576</t>
+        </is>
+      </c>
+      <c r="H21" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+      <c r="I21" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+      <c r="J21" s="0" t="inlineStr">
+        <is>
+          <t>ms</t>
+        </is>
+      </c>
+      <c r="K21" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+      <c r="L21" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="inlineStr">
+        <is>
+          <t>4.245</t>
+        </is>
+      </c>
+      <c r="B22" s="0" t="inlineStr">
+        <is>
+          <t>2.704</t>
+        </is>
+      </c>
+      <c r="C22" s="0" t="inlineStr">
+        <is>
+          <t>1.808</t>
+        </is>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>3.268</t>
+        </is>
+      </c>
+      <c r="E22" s="0" t="inlineStr">
+        <is>
+          <t>2.565</t>
+        </is>
+      </c>
+      <c r="F22" s="0" t="inlineStr">
+        <is>
+          <t>2097152</t>
+        </is>
+      </c>
+      <c r="H22" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+      <c r="I22" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+      <c r="J22" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+      <c r="K22" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+      <c r="L22" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="inlineStr">
+        <is>
+          <t>8.303</t>
+        </is>
+      </c>
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>5.328</t>
+        </is>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>4.139</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>6.798</t>
+        </is>
+      </c>
+      <c r="E23" s="0" t="inlineStr">
+        <is>
+          <t>5.324</t>
+        </is>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>4194304</t>
+        </is>
+      </c>
+      <c r="H23" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+      <c r="I23" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+      <c r="J23" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+      <c r="K23" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
+        </is>
+      </c>
+      <c r="L23" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s</t>
         </is>
       </c>
     </row>

</xml_diff>